<commit_message>
Actualizar archivo de productos.xlsx
</commit_message>
<xml_diff>
--- a/productos/productos.xlsx
+++ b/productos/productos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugeniovazquez\Desktop\Nueva carpeta (3)\productos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugeniovazquez\Desktop\Nueva carpeta (3) - copia\productos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="135">
   <si>
     <t>Familia</t>
   </si>
@@ -44,9 +44,6 @@
     <t>COSTO FINAL CON PROMO</t>
   </si>
   <si>
-    <t xml:space="preserve">EDP BOOS INTENSE WOMAN </t>
-  </si>
-  <si>
     <t xml:space="preserve">EAU DE PARFUM BOOS BLACK EXTREME </t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>PACK STAY TRUE BODY + DEO</t>
   </si>
   <si>
-    <t>PACK STAY WILD BODY + DEO</t>
-  </si>
-  <si>
     <t>PACK MUAA STAY REAL COLONIA BODY CREAM</t>
   </si>
   <si>
@@ -227,54 +221,9 @@
     <t>PACK MUAA STAY WILD COLONIA BODY CREAM</t>
   </si>
   <si>
-    <t>BOOS NECESER FOREVER EDP 100 ML + DEO 127 ML</t>
-  </si>
-  <si>
-    <t>BOOS NECESER MIDNIGHT EDP 100 ML + DEO 127 ML</t>
-  </si>
-  <si>
-    <t>BOOS NECESER RAINBOW EDP 100 ML + DEO 127 ML</t>
-  </si>
-  <si>
-    <t>BOOS NECESER INTENSE WOMAN  EDP 90 ML + DEO 127 ML</t>
-  </si>
-  <si>
-    <t>BOOS NECESER INTENSE WOMAN LUMIERE EDP 90 ML + DEO 127 ML</t>
-  </si>
-  <si>
-    <t>BOOS NECESER INTENSE WOMAN ROSE EDP 90 ML + DEO 127 ML</t>
-  </si>
-  <si>
     <t>BOOS NECESER INTENSE ATTRACTION WOMAN EDP+DEO</t>
   </si>
   <si>
-    <t>Pack Eau de Parfum Rainbow 100 ml + Deo de regalo</t>
-  </si>
-  <si>
-    <t>Pack Eau de Parfum Midnight 100 ml + Deo de regalo</t>
-  </si>
-  <si>
-    <t>Pack Eau de Parfum Intense Woman 90 ml + Deo de regalo</t>
-  </si>
-  <si>
-    <t>Pack Eau de Parfum Intense Woman Lumiere 90 ml + Deo de regalo</t>
-  </si>
-  <si>
-    <t>Pack Eau de Parfum Intense Rosé 90 ml + Deo de regalo</t>
-  </si>
-  <si>
-    <t>Pack Boos EDP Intense Attraction woman + Deo de regalo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACK TOTE SHINE CLASSIC EDP+DEO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACK TOTE SHINE GOLDEN R EDP+DEO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACK TOTE SHINE RUBY ELIXIR </t>
-  </si>
-  <si>
     <t>Pack WELLINGTON  FEMENINO ROSA edp + Deo de regalo</t>
   </si>
   <si>
@@ -299,30 +248,12 @@
     <t>BOOS NECESER INTENSE ATTRACTION EDP 90 ML +DEO 150 ML</t>
   </si>
   <si>
-    <t>PACK DEO REGALO BOOS ACQUA</t>
-  </si>
-  <si>
     <t xml:space="preserve">PACK DEO REGALO BOOS BLACK </t>
   </si>
   <si>
     <t>PACK DEO REGALO BOOS RED</t>
   </si>
   <si>
-    <t xml:space="preserve">WELLINGTON POLO CLUB NECESER RED EDP 90 ml +DEO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WELLINGTON POLO CLUB NECESER BLACK EDP 90 ml +DEO </t>
-  </si>
-  <si>
-    <t>WELLINGTON POLO CLUB EDP 90 ml +DEO BLUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WELLINGTON POLO CLUB NECESER LEGEND  EDP 90 ml +DEO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WELLINGTON POLO CLUB NECESER LEGEND SPIRIT  EDP 90 ml +DEO </t>
-  </si>
-  <si>
     <t>BOOS DEO HOMBRE</t>
   </si>
   <si>
@@ -483,6 +414,21 @@
   </si>
   <si>
     <t>MUA DEO STAY WILD DEO MUA x6un</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGTN POLO CLUB NECESER RED EDP 90 ml +DEO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGTN POLO CLUB NECESER BLACK EDP 90 ml +DEO </t>
+  </si>
+  <si>
+    <t>WGTN POLO CLUB EDP 90 ml +DEO BLUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGTN POLO CLUB NECESER LEGEND  EDP 90 ml +DEO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGTN POLO CLUB NECESER LEGEND SPIRIT  EDP 90 ml +DEO </t>
   </si>
 </sst>
 </file>
@@ -662,7 +608,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -877,17 +823,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -899,7 +834,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -978,7 +913,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1041,9 +975,6 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1054,12 +985,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="15" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1086,7 +1011,62 @@
     <cellStyle name="Normal 6 2" xfId="3"/>
     <cellStyle name="Normal_Wella precios Oct 2009- lista 27" xfId="1"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="57">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1105,106 +1085,6 @@
     <dxf>
       <font>
         <color rgb="FFBFBFBF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFBFBFBF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFBFBFBF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
@@ -1693,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,13 +1610,13 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6">
@@ -1748,13 +1628,13 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6">
@@ -1766,13 +1646,13 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6">
@@ -1784,13 +1664,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6">
@@ -1802,13 +1682,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6">
@@ -1820,13 +1700,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="6">
@@ -1838,13 +1718,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="6">
@@ -1856,13 +1736,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="6">
@@ -1874,13 +1754,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6">
@@ -1892,13 +1772,13 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="6">
@@ -1910,13 +1790,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="6">
@@ -1928,13 +1808,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="6">
@@ -1946,13 +1826,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="6">
@@ -1964,13 +1844,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="6">
@@ -1982,10 +1862,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="7"/>
@@ -1994,10 +1874,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="7"/>
@@ -2006,22 +1886,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="7"/>
@@ -2030,10 +1910,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>7</v>
+        <v>84</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="7"/>
@@ -2042,10 +1922,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="7"/>
@@ -2054,10 +1934,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>8</v>
+        <v>84</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>82</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="7"/>
@@ -2066,10 +1946,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="7"/>
@@ -2078,10 +1958,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="7"/>
@@ -2090,21 +1970,21 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="12"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="4"/>
@@ -2114,9 +1994,9 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="4"/>
@@ -2126,9 +2006,9 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="4"/>
@@ -2138,7 +2018,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>13</v>
@@ -2150,9 +2030,9 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B30" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="4"/>
@@ -2162,7 +2042,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>15</v>
@@ -2174,9 +2054,9 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="4"/>
@@ -2186,9 +2066,9 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C33" s="4"/>
@@ -2198,21 +2078,21 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="13"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B35" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="4"/>
@@ -2222,9 +2102,9 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="4"/>
@@ -2234,9 +2114,9 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="29" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="4"/>
@@ -2246,9 +2126,9 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B38" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C38" s="4"/>
@@ -2258,9 +2138,9 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="4"/>
@@ -2270,9 +2150,9 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="4"/>
@@ -2282,9 +2162,9 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B41" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="4"/>
@@ -2294,7 +2174,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B42" s="22" t="s">
         <v>26</v>
@@ -2306,9 +2186,9 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C43" s="4"/>
@@ -2318,9 +2198,9 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="4"/>
@@ -2330,9 +2210,9 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B45" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C45" s="4"/>
@@ -2342,9 +2222,9 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B46" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="4"/>
@@ -2354,10 +2234,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B47" s="32" t="s">
-        <v>31</v>
+        <v>88</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="7"/>
@@ -2366,10 +2246,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="7"/>
@@ -2378,10 +2258,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>136</v>
+        <v>88</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="7"/>
@@ -2390,10 +2270,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="7"/>
@@ -2402,10 +2282,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="7"/>
@@ -2414,10 +2294,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="7"/>
@@ -2426,10 +2306,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" s="22" t="s">
-        <v>140</v>
+        <v>88</v>
+      </c>
+      <c r="B53" s="32" t="s">
+        <v>118</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="7"/>
@@ -2438,22 +2318,22 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B54" s="33" t="s">
-        <v>141</v>
+        <v>88</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="C54" s="4"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="12"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="11"/>
       <c r="F54" s="19"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>142</v>
+        <v>88</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>120</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -2462,10 +2342,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B56" s="28" t="s">
-        <v>143</v>
+        <v>93</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -2474,10 +2354,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -2486,10 +2366,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>145</v>
+        <v>93</v>
+      </c>
+      <c r="B58" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -2498,9 +2378,9 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B59" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="33" t="s">
         <v>32</v>
       </c>
       <c r="C59" s="4"/>
@@ -2510,9 +2390,9 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B60" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="33" t="s">
         <v>33</v>
       </c>
       <c r="C60" s="4"/>
@@ -2522,10 +2402,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -2534,10 +2414,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B62" s="35" t="s">
-        <v>146</v>
+        <v>94</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>124</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -2546,10 +2426,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B63" s="35" t="s">
-        <v>147</v>
+        <v>94</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>125</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -2558,10 +2438,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B64" s="35" t="s">
-        <v>148</v>
+        <v>94</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>126</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -2570,19 +2450,19 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B65" s="35" t="s">
-        <v>149</v>
+        <v>94</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>34</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="11"/>
       <c r="F65" s="19"/>
     </row>
-    <row r="66" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B66" s="35" t="s">
         <v>35</v>
@@ -2594,7 +2474,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B67" s="36" t="s">
         <v>36</v>
@@ -2604,11 +2484,11 @@
       <c r="E67" s="11"/>
       <c r="F67" s="19"/>
     </row>
-    <row r="68" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B68" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C68" s="4"/>
@@ -2616,11 +2496,11 @@
       <c r="E68" s="11"/>
       <c r="F68" s="19"/>
     </row>
-    <row r="69" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B69" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B69" s="34" t="s">
         <v>38</v>
       </c>
       <c r="C69" s="4"/>
@@ -2630,9 +2510,9 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B70" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="37" t="s">
         <v>39</v>
       </c>
       <c r="C70" s="4"/>
@@ -2642,9 +2522,9 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B71" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C71" s="4"/>
@@ -2652,35 +2532,35 @@
       <c r="E71" s="11"/>
       <c r="F71" s="19"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B72" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="11"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="17"/>
       <c r="F72" s="19"/>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B73" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="17"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="15"/>
       <c r="F73" s="19"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B74" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B74" s="34" t="s">
         <v>43</v>
       </c>
       <c r="C74" s="14"/>
@@ -2690,9 +2570,9 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B75" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C75" s="14"/>
@@ -2702,9 +2582,9 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B76" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="34" t="s">
         <v>45</v>
       </c>
       <c r="C76" s="14"/>
@@ -2714,9 +2594,9 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B77" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" s="38" t="s">
         <v>46</v>
       </c>
       <c r="C77" s="14"/>
@@ -2726,9 +2606,9 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B78" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C78" s="14"/>
@@ -2738,9 +2618,9 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B79" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B79" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C79" s="14"/>
@@ -2750,9 +2630,9 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B80" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B80" s="38" t="s">
         <v>49</v>
       </c>
       <c r="C80" s="14"/>
@@ -2762,7 +2642,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="B81" s="39" t="s">
         <v>50</v>
@@ -2774,33 +2654,33 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B82" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C82" s="14"/>
+      <c r="C82" s="10"/>
       <c r="D82" s="10"/>
       <c r="E82" s="15"/>
       <c r="F82" s="19"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B83" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B83" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C83" s="10"/>
+      <c r="C83" s="14"/>
       <c r="D83" s="10"/>
       <c r="E83" s="15"/>
       <c r="F83" s="19"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B84" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" s="39" t="s">
         <v>53</v>
       </c>
       <c r="C84" s="14"/>
@@ -2810,31 +2690,31 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B85" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C85" s="14"/>
+      <c r="C85" s="10"/>
       <c r="D85" s="10"/>
       <c r="E85" s="15"/>
       <c r="F85" s="19"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B86" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C86" s="10"/>
+      <c r="C86" s="14"/>
       <c r="D86" s="10"/>
       <c r="E86" s="15"/>
       <c r="F86" s="19"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B87" s="42" t="s">
         <v>56</v>
@@ -2846,31 +2726,31 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B88" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C88" s="14"/>
+      <c r="C88" s="10"/>
       <c r="D88" s="10"/>
       <c r="E88" s="15"/>
       <c r="F88" s="19"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B89" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C89" s="10"/>
+      <c r="C89" s="14"/>
       <c r="D89" s="10"/>
       <c r="E89" s="15"/>
       <c r="F89" s="19"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B90" s="44" t="s">
         <v>59</v>
@@ -2880,59 +2760,59 @@
       <c r="E90" s="15"/>
       <c r="F90" s="19"/>
     </row>
-    <row r="91" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B91" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="C91" s="14"/>
+        <v>127</v>
+      </c>
+      <c r="C91" s="10"/>
       <c r="D91" s="10"/>
       <c r="E91" s="15"/>
       <c r="F91" s="19"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B92" s="46" t="s">
-        <v>150</v>
+        <v>98</v>
+      </c>
+      <c r="B92" s="43" t="s">
+        <v>128</v>
       </c>
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
       <c r="E92" s="15"/>
       <c r="F92" s="19"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B93" s="44" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
       <c r="E93" s="15"/>
       <c r="F93" s="19"/>
     </row>
-    <row r="94" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B94" s="45" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
       <c r="E94" s="15"/>
       <c r="F94" s="19"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B95" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" s="43" t="s">
         <v>61</v>
       </c>
       <c r="C95" s="10"/>
@@ -2942,9 +2822,9 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B96" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C96" s="10"/>
@@ -2952,9 +2832,9 @@
       <c r="E96" s="15"/>
       <c r="F96" s="19"/>
     </row>
-    <row r="97" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B97" s="47" t="s">
         <v>63</v>
@@ -2966,7 +2846,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B98" s="48" t="s">
         <v>64</v>
@@ -2978,7 +2858,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B99" s="49" t="s">
         <v>65</v>
@@ -2990,652 +2870,407 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B100" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="15"/>
-      <c r="F100" s="19"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B101" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="15"/>
-      <c r="F101" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="B101" s="50" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B102" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="15"/>
-      <c r="F102" s="19"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="B102" s="50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="B103" s="51" t="s">
-        <v>69</v>
-      </c>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="15"/>
-      <c r="F103" s="19"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B104" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
-      <c r="E104" s="15"/>
-      <c r="F104" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="B104" s="54" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B105" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="15"/>
-      <c r="F105" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="B105" s="54" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B106" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="15"/>
-      <c r="F106" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="B106" s="54" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B107" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
-      <c r="E107" s="15"/>
-      <c r="F107" s="19"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="B107" s="54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B108" s="51" t="s">
-        <v>80</v>
+        <v>99</v>
+      </c>
+      <c r="B108" s="54" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B109" s="51" t="s">
-        <v>81</v>
+        <v>100</v>
+      </c>
+      <c r="B109" s="53" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B110" s="53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="B110" s="52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B111" s="54" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="B111" s="49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B112" s="54" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="B112" s="49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B113" s="54" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="B113" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B114" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B115" s="58" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B116" s="58" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B117" s="58" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A118" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B118" s="58" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A119" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B119" s="58" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B120" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="C120" s="10"/>
-      <c r="D120" s="10"/>
-      <c r="E120" s="15"/>
-      <c r="F120" s="19"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B121" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
-      <c r="E121" s="15"/>
-      <c r="F121" s="19"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B122" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-      <c r="E122" s="15"/>
-      <c r="F122" s="19"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B123" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="15"/>
-      <c r="F123" s="19"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B124" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="15"/>
-      <c r="F124" s="19"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B125" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="19"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B126" s="56" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B127" s="57" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B128" s="56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B129" s="51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B130" s="51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B131" s="51" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B132" s="51" t="s">
-        <v>86</v>
+        <v>100</v>
+      </c>
+      <c r="B114" s="49" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A9 C43:D44 B46 C46:D48 A37:A48">
-    <cfRule type="expression" dxfId="65" priority="52">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7 A26 D7">
-    <cfRule type="expression" dxfId="64" priority="53">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50:D50 C52:D53 D51">
-    <cfRule type="expression" dxfId="63" priority="72">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10:B11 B6 D8:D11 D6">
-    <cfRule type="expression" dxfId="62" priority="71">
+  <conditionalFormatting sqref="A9 C42:D43 B45 C45:D47 A36:A47">
+    <cfRule type="expression" dxfId="56" priority="52">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7 A25 D7">
+    <cfRule type="expression" dxfId="55" priority="53">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:D49 C51:D52 D50">
+    <cfRule type="expression" dxfId="54" priority="72">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B11 B6 D8:D11 D6 A17:A24 B96:B97 B99 A74:A103 A109:A114">
+    <cfRule type="expression" dxfId="53" priority="71">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 D5 B8:B9">
-    <cfRule type="expression" dxfId="61" priority="70">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B14 B17:B18 C16:D18 A16 D13:D15">
-    <cfRule type="expression" dxfId="60" priority="67">
+    <cfRule type="expression" dxfId="52" priority="70">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B14 B17 C16:D17 A16 D13:D15">
+    <cfRule type="expression" dxfId="51" priority="67">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12 D12 B15">
-    <cfRule type="expression" dxfId="59" priority="66">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36:B37 B43:B44 B50:B51 B40:B41 B47:B48 C36:D41">
-    <cfRule type="expression" dxfId="58" priority="64">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35 B42 B49 D35 D42 D49 B38:B39 B52:B53">
-    <cfRule type="expression" dxfId="57" priority="63">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35 C42 C49">
-    <cfRule type="expression" dxfId="56" priority="62">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:B21 B24:B25 C20:D25">
-    <cfRule type="expression" dxfId="55" priority="61">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19 D19 B22:B23">
-    <cfRule type="expression" dxfId="54" priority="60">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="53" priority="59">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="52" priority="58">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="51" priority="56">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:D54">
-    <cfRule type="expression" dxfId="50" priority="57">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B27 B29:B30 B32:B33 C26:D34 A26">
-    <cfRule type="expression" dxfId="49" priority="55">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28 B31 B34">
-    <cfRule type="expression" dxfId="48" priority="54">
+    <cfRule type="expression" dxfId="50" priority="66">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:B36 B42:B43 B49:B50 B39:B40 B46:B47 C35:D40">
+    <cfRule type="expression" dxfId="49" priority="64">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34 B41 B48 D34 D41 D48 B37:B38 B51:B52">
+    <cfRule type="expression" dxfId="48" priority="63">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34 C41 C48">
+    <cfRule type="expression" dxfId="47" priority="62">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:B20 B23:B24 C19:D24">
+    <cfRule type="expression" dxfId="46" priority="61">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18 D18 B21:B22">
+    <cfRule type="expression" dxfId="45" priority="60">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="44" priority="59">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="43" priority="58">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="expression" dxfId="42" priority="56">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53:D53">
+    <cfRule type="expression" dxfId="41" priority="57">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:B26 B28:B29 B31:B32 C25:D33 A25">
+    <cfRule type="expression" dxfId="40" priority="55">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27 B30 B33">
+    <cfRule type="expression" dxfId="39" priority="54">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="47" priority="73">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B73:D73 B55:D56 A57:D62 B63:D64">
-    <cfRule type="expression" dxfId="46" priority="51">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16:E18">
-    <cfRule type="expression" dxfId="45" priority="50">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E25">
-    <cfRule type="expression" dxfId="44" priority="49">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E34">
-    <cfRule type="expression" dxfId="43" priority="48">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35:E54">
-    <cfRule type="expression" dxfId="42" priority="47">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E55:E57 E73">
-    <cfRule type="expression" dxfId="41" priority="46">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="40" priority="45">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="39" priority="44">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="38" priority="43">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82:B83 B89:B90 B86:B87 B102:B105 B96 B93:B94">
-    <cfRule type="expression" dxfId="37" priority="42">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B81 B88 B95 B74 B84:B85 B91:B92 B100:B101 B106:B107">
-    <cfRule type="expression" dxfId="36" priority="41">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B75:B80">
-    <cfRule type="expression" dxfId="35" priority="40">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B97:B99">
-    <cfRule type="expression" dxfId="34" priority="39">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C74:C80">
-    <cfRule type="expression" dxfId="33" priority="38">
+    <cfRule type="expression" dxfId="38" priority="73">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B72:D72 B54:D55 A56:D61 B62:D63">
+    <cfRule type="expression" dxfId="37" priority="51">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E17 E73:E99">
+    <cfRule type="expression" dxfId="36" priority="50">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E24">
+    <cfRule type="expression" dxfId="35" priority="49">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E33">
+    <cfRule type="expression" dxfId="34" priority="48">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:E53">
+    <cfRule type="expression" dxfId="33" priority="47">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54:E56 E72">
+    <cfRule type="expression" dxfId="32" priority="46">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" dxfId="31" priority="45">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" dxfId="30" priority="44">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="29" priority="43">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B81:B82 B88:B89 B85:B86 B95 B92:B93">
+    <cfRule type="expression" dxfId="28" priority="42">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B80 B87 B94 B73 B83:B84 B90:B91 B98">
+    <cfRule type="expression" dxfId="27" priority="41">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74:B79">
+    <cfRule type="expression" dxfId="26" priority="40">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73:C79">
+    <cfRule type="expression" dxfId="25" priority="38">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C80">
+    <cfRule type="expression" dxfId="24" priority="37">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C83">
+    <cfRule type="expression" dxfId="23" priority="36">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C86">
+    <cfRule type="expression" dxfId="22" priority="35">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C89">
+    <cfRule type="expression" dxfId="21" priority="34">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="expression" dxfId="32" priority="37">
+    <cfRule type="expression" dxfId="20" priority="33">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="expression" dxfId="31" priority="36">
+    <cfRule type="expression" dxfId="19" priority="32">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="expression" dxfId="30" priority="35">
+    <cfRule type="expression" dxfId="18" priority="31">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="29" priority="34">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82">
-    <cfRule type="expression" dxfId="28" priority="33">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
-    <cfRule type="expression" dxfId="27" priority="32">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C88">
-    <cfRule type="expression" dxfId="26" priority="31">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91">
-    <cfRule type="expression" dxfId="25" priority="30">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E74:E107">
-    <cfRule type="expression" dxfId="24" priority="29">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75:A114">
-    <cfRule type="expression" dxfId="23" priority="28">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:D70 B65:D69 B71:D72">
-    <cfRule type="expression" dxfId="22" priority="27">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65:E72">
-    <cfRule type="expression" dxfId="21" priority="26">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E64">
-    <cfRule type="expression" dxfId="20" priority="24">
+    <cfRule type="expression" dxfId="17" priority="30">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69:D69 B64:D68 B70:D71">
+    <cfRule type="expression" dxfId="16" priority="27">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64:E71">
+    <cfRule type="expression" dxfId="15" priority="26">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57:E63">
+    <cfRule type="expression" dxfId="14" priority="24">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="13" priority="20">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B4 D2:D4">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="12" priority="19">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="10" priority="17">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A8">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="9" priority="16">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A8">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="8" priority="15">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A15">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:A25">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A36">
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A36">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49:A56">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="7" priority="14">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A35">
+    <cfRule type="expression" dxfId="6" priority="11">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A35">
+    <cfRule type="expression" dxfId="5" priority="12">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:A55">
+    <cfRule type="expression" dxfId="4" priority="10">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C15">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:A69">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:A74">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B120:B121 B123:B124">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B122 B125">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E120:E125">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A120:A125">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A115:A119">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>#REF!="SIN STOCK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A126:A132">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="9">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:A68">
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:A73">
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>#REF!="SIN STOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104:A108">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>#REF!="SIN STOCK"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>